<commit_message>
list view does not work properly
</commit_message>
<xml_diff>
--- a/AstronomicalProcessingProject/Resources/Book1.xlsx
+++ b/AstronomicalProcessingProject/Resources/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tafewa-my.sharepoint.com/personal/30065695_tafe_wa_edu_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\30065695\Source\Repos\AstronomicalProcessingProject\AstronomicalProcessingProject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8A3CEEB-490A-4C89-9DF0-B3830EB98491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DFCFE1-CCEA-4C55-8FE0-F71CEF19095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD22024D-09C0-485B-BA60-299F93782DFD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{BD22024D-09C0-485B-BA60-299F93782DFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>EN</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>Radiobuttons</t>
+  </si>
+  <si>
+    <t>Astronomical Processing</t>
+  </si>
+  <si>
+    <t>Astronomische Verarbeitung</t>
+  </si>
+  <si>
+    <t>Traitement astronomique</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCA10E7-2B43-431E-AB49-A90A91F82383}">
-  <dimension ref="C3:F21"/>
+  <dimension ref="C3:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,209 +593,220 @@
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>